<commit_message>
Ultima que soy bobo
</commit_message>
<xml_diff>
--- a/P4/cuestionario-SUS.xlsx
+++ b/P4/cuestionario-SUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josej\Desktop\universidad\3º\2ºcuatri\DIU\DIU-git\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0C790D-9183-4616-BBF2-2765FB970D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66004DFF-F1A9-4412-BFE6-EB03A531BC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1009,6 +1009,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,14 +1020,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1262,8 +1262,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1408,37 +1408,37 @@
       <c r="B9" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="63" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="65" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="49"/>
-      <c r="C10" s="62"/>
+      <c r="C10" s="63"/>
       <c r="D10" s="29"/>
       <c r="E10" s="64"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="36"/>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
@@ -1482,7 +1482,7 @@
       <c r="F13" s="17">
         <v>3</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="59">
         <v>2</v>
       </c>
       <c r="H13" s="14"/>
@@ -1507,7 +1507,7 @@
       <c r="F14" s="17">
         <v>1</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="59">
         <v>3</v>
       </c>
       <c r="H14" s="14"/>
@@ -1532,7 +1532,7 @@
       <c r="F15" s="17">
         <v>5</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="59">
         <v>3</v>
       </c>
       <c r="H15" s="14"/>
@@ -1556,7 +1556,7 @@
       <c r="F16" s="17">
         <v>1</v>
       </c>
-      <c r="G16" s="65">
+      <c r="G16" s="59">
         <v>4</v>
       </c>
       <c r="H16" s="14"/>
@@ -1580,7 +1580,7 @@
       <c r="F17" s="17">
         <v>3</v>
       </c>
-      <c r="G17" s="65">
+      <c r="G17" s="59">
         <v>4</v>
       </c>
       <c r="H17" s="14"/>
@@ -1604,7 +1604,7 @@
       <c r="F18" s="53">
         <v>2</v>
       </c>
-      <c r="G18" s="65">
+      <c r="G18" s="59">
         <v>2</v>
       </c>
       <c r="H18" s="14"/>
@@ -1628,7 +1628,7 @@
       <c r="F19" s="17">
         <v>5</v>
       </c>
-      <c r="G19" s="65">
+      <c r="G19" s="59">
         <v>3</v>
       </c>
       <c r="H19" s="14"/>
@@ -1652,7 +1652,7 @@
       <c r="F20" s="17">
         <v>1</v>
       </c>
-      <c r="G20" s="65">
+      <c r="G20" s="59">
         <v>3</v>
       </c>
       <c r="H20" s="14"/>
@@ -1676,7 +1676,7 @@
       <c r="F21" s="17">
         <v>5</v>
       </c>
-      <c r="G21" s="65">
+      <c r="G21" s="59">
         <v>2</v>
       </c>
       <c r="H21" s="14"/>
@@ -1700,7 +1700,7 @@
       <c r="F22" s="17">
         <v>1</v>
       </c>
-      <c r="G22" s="65">
+      <c r="G22" s="59">
         <v>3</v>
       </c>
       <c r="H22" s="14"/>
@@ -1743,13 +1743,13 @@
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="22" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F24" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="22" t="s">
-        <v>60</v>
+      <c r="G24" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2789,6 +2789,6 @@
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="72" fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>